<commit_message>
* Add committee and key dates
</commit_message>
<xml_diff>
--- a/data/committee.xlsx
+++ b/data/committee.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\widmelu1\Downloads\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D6D18B-6272-4F72-A8D8-146E347D134E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DD412E-F42D-48F4-AC82-6D5DABCB6D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12000" yWindow="5205" windowWidth="21930" windowHeight="11730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8055" yWindow="6135" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
   <si>
     <t>First</t>
   </si>
@@ -45,16 +45,238 @@
     <t>local</t>
   </si>
   <si>
-    <t>TBD</t>
-  </si>
-  <si>
-    <t>Executive</t>
-  </si>
-  <si>
-    <t>Scientific</t>
-  </si>
-  <si>
-    <t>Local</t>
+    <t>Arne</t>
+  </si>
+  <si>
+    <t>Bathke</t>
+  </si>
+  <si>
+    <t>University of Salzburg</t>
+  </si>
+  <si>
+    <t>Werner</t>
+  </si>
+  <si>
+    <t>Brannath</t>
+  </si>
+  <si>
+    <t>University of Bremen</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>Bretz</t>
+  </si>
+  <si>
+    <t>Novartis</t>
+  </si>
+  <si>
+    <t>Uli</t>
+  </si>
+  <si>
+    <t>Burger</t>
+  </si>
+  <si>
+    <t>Roche</t>
+  </si>
+  <si>
+    <t>Malgorzata</t>
+  </si>
+  <si>
+    <t>Graczyk</t>
+  </si>
+  <si>
+    <t>Poznań University of Life Sciences</t>
+  </si>
+  <si>
+    <t>Annette</t>
+  </si>
+  <si>
+    <t>Kopp-Schneider</t>
+  </si>
+  <si>
+    <t>German Cancer Research Center</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Berghold</t>
+  </si>
+  <si>
+    <t>Medical University of Graz</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Beyersmann</t>
+  </si>
+  <si>
+    <t>University of Ulm</t>
+  </si>
+  <si>
+    <t>Harald</t>
+  </si>
+  <si>
+    <t>Binder</t>
+  </si>
+  <si>
+    <t>University of Freiburg</t>
+  </si>
+  <si>
+    <t>Anne-Laure</t>
+  </si>
+  <si>
+    <t>Boulesteix</t>
+  </si>
+  <si>
+    <t>University of Munich</t>
+  </si>
+  <si>
+    <t>Tomasz</t>
+  </si>
+  <si>
+    <t>Burzykowski</t>
+  </si>
+  <si>
+    <t>Hasselt University</t>
+  </si>
+  <si>
+    <t>Vanessa</t>
+  </si>
+  <si>
+    <t>Didelez</t>
+  </si>
+  <si>
+    <t>Janusz</t>
+  </si>
+  <si>
+    <t>Gołaszewski</t>
+  </si>
+  <si>
+    <t>University of Warmia and Mazury in Olsztyn</t>
+  </si>
+  <si>
+    <t>Dominik</t>
+  </si>
+  <si>
+    <t>Heinzmann</t>
+  </si>
+  <si>
+    <t>Novo Nordisk</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Hofner</t>
+  </si>
+  <si>
+    <t>Paul-Ehrlich-Institut</t>
+  </si>
+  <si>
+    <t>Shu-Fang</t>
+  </si>
+  <si>
+    <t>Hsu Schmitz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Janssen </t>
+  </si>
+  <si>
+    <t>Agnieszka</t>
+  </si>
+  <si>
+    <t>Kubik-Komar</t>
+  </si>
+  <si>
+    <t>University of Life Sciences in Lubli</t>
+  </si>
+  <si>
+    <t>Dominic</t>
+  </si>
+  <si>
+    <t>Magirr</t>
+  </si>
+  <si>
+    <t>Valentin</t>
+  </si>
+  <si>
+    <t>Rousson</t>
+  </si>
+  <si>
+    <t>University of Lausanne</t>
+  </si>
+  <si>
+    <t>Susanne</t>
+  </si>
+  <si>
+    <t>Strohmaier</t>
+  </si>
+  <si>
+    <t>Medical University of Vienna</t>
+  </si>
+  <si>
+    <t>Laurence</t>
+  </si>
+  <si>
+    <t>Giullier</t>
+  </si>
+  <si>
+    <t>Tracy</t>
+  </si>
+  <si>
+    <t>Glass</t>
+  </si>
+  <si>
+    <t>University of Basel</t>
+  </si>
+  <si>
+    <t>Achim</t>
+  </si>
+  <si>
+    <t>Güttner</t>
+  </si>
+  <si>
+    <t>Eliane</t>
+  </si>
+  <si>
+    <t>Imfeld</t>
+  </si>
+  <si>
+    <t>Giusi</t>
+  </si>
+  <si>
+    <t>Moffa</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>Sorensson</t>
+  </si>
+  <si>
+    <t>Xcenda</t>
+  </si>
+  <si>
+    <t>Kristina</t>
+  </si>
+  <si>
+    <t>Weber</t>
+  </si>
+  <si>
+    <t>Lukas</t>
+  </si>
+  <si>
+    <t>Widmer</t>
+  </si>
+  <si>
+    <t>Marcel</t>
+  </si>
+  <si>
+    <t>Wolbers</t>
   </si>
 </sst>
 </file>
@@ -372,17 +594,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
@@ -409,27 +631,33 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>11</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -437,15 +665,397 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
       <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>67</v>
+      </c>
+      <c r="C23" t="s">
+        <v>68</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" t="s">
+        <v>70</v>
+      </c>
+      <c r="C24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>68</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>80</v>
+      </c>
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
* FB> editorial changes *
</commit_message>
<xml_diff>
--- a/data/committee.xlsx
+++ b/data/committee.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\widmelu1\Downloads\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEN2023\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DD412E-F42D-48F4-AC82-6D5DABCB6D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A94431-CC27-43FB-97E5-3A105DF5A9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8055" yWindow="6135" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1590" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
   <si>
     <t>First</t>
   </si>
@@ -255,9 +255,6 @@
     <t>Fred</t>
   </si>
   <si>
-    <t>Sorensson</t>
-  </si>
-  <si>
     <t>Xcenda</t>
   </si>
   <si>
@@ -277,6 +274,15 @@
   </si>
   <si>
     <t>Wolbers</t>
+  </si>
+  <si>
+    <t>Leibniz Institute for Prevention Research and Epidemiology - BIPS, Bremen</t>
+  </si>
+  <si>
+    <t>Swiss Tropical and Public Health Institute</t>
+  </si>
+  <si>
+    <t>Sorenson</t>
   </si>
 </sst>
 </file>
@@ -597,7 +603,7 @@
   <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +821,7 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>11</v>
+        <v>83</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -955,7 +961,7 @@
         <v>67</v>
       </c>
       <c r="C23" t="s">
-        <v>68</v>
+        <v>84</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -1008,10 +1014,10 @@
         <v>75</v>
       </c>
       <c r="B27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C27" t="s">
         <v>76</v>
-      </c>
-      <c r="C27" t="s">
-        <v>77</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1019,10 +1025,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28" t="s">
         <v>78</v>
-      </c>
-      <c r="B28" t="s">
-        <v>79</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
@@ -1033,10 +1039,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
         <v>80</v>
-      </c>
-      <c r="B29" t="s">
-        <v>81</v>
       </c>
       <c r="C29" t="s">
         <v>14</v>
@@ -1047,10 +1053,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
         <v>82</v>
-      </c>
-      <c r="B30" t="s">
-        <v>83</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
* Add call for short courses * Update Committee
</commit_message>
<xml_diff>
--- a/data/committee.xlsx
+++ b/data/committee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEN2023\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\widmelu1\Downloads\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19A94431-CC27-43FB-97E5-3A105DF5A9BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF188C6-4D24-4F3C-A983-EA440D29311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1590" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8070" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="89">
   <si>
     <t>First</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Kubik-Komar</t>
   </si>
   <si>
-    <t>University of Life Sciences in Lubli</t>
-  </si>
-  <si>
     <t>Dominic</t>
   </si>
   <si>
@@ -283,6 +280,18 @@
   </si>
   <si>
     <t>Sorenson</t>
+  </si>
+  <si>
+    <t>University of Life Sciences in Lublin</t>
+  </si>
+  <si>
+    <t>Lilla</t>
+  </si>
+  <si>
+    <t>Di Scala</t>
+  </si>
+  <si>
+    <t>Johnson &amp; Johnson</t>
   </si>
 </sst>
 </file>
@@ -600,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +830,7 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -891,7 +900,7 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>85</v>
       </c>
       <c r="E18">
         <v>1</v>
@@ -899,10 +908,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
         <v>56</v>
-      </c>
-      <c r="B19" t="s">
-        <v>57</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
@@ -913,13 +922,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>59</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
       </c>
       <c r="E20">
         <v>1</v>
@@ -927,13 +936,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>62</v>
-      </c>
-      <c r="C21" t="s">
-        <v>63</v>
       </c>
       <c r="E21">
         <v>1</v>
@@ -941,27 +950,24 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="F23">
         <v>1</v>
@@ -969,13 +975,13 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C24" t="s">
-        <v>14</v>
+        <v>83</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -983,10 +989,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -997,13 +1003,13 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C26" t="s">
-        <v>68</v>
+        <v>14</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1011,13 +1017,13 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1025,13 +1031,13 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>75</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1039,13 +1045,13 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1053,15 +1059,29 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" t="s">
+        <v>79</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" t="s">
         <v>81</v>
       </c>
-      <c r="B30" t="s">
-        <v>82</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>17</v>
       </c>
-      <c r="F30">
+      <c r="F31">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FB> minor editorial changes
</commit_message>
<xml_diff>
--- a/data/committee.xlsx
+++ b/data/committee.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\widmelu1\Downloads\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEN2023\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF188C6-4D24-4F3C-A983-EA440D29311E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E249BE4-D63D-482E-A89A-9DF59C1D6416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8070" yWindow="2550" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,6 +958,9 @@
       <c r="C22" t="s">
         <v>88</v>
       </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">

</xml_diff>

<commit_message>
* Fix typo on committee page
</commit_message>
<xml_diff>
--- a/data/committee.xlsx
+++ b/data/committee.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CEN2023\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\widmelu1\Downloads\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E249BE4-D63D-482E-A89A-9DF59C1D6416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398696B2-95AA-4F8E-8205-E0EE301885A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-27480" yWindow="1320" windowWidth="21600" windowHeight="11190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>Laurence</t>
   </si>
   <si>
-    <t>Giullier</t>
-  </si>
-  <si>
     <t>Tracy</t>
   </si>
   <si>
@@ -292,6 +289,9 @@
   </si>
   <si>
     <t>Johnson &amp; Johnson</t>
+  </si>
+  <si>
+    <t>Guillier</t>
   </si>
 </sst>
 </file>
@@ -611,20 +611,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="22.5703125" customWidth="1"/>
-    <col min="2" max="2" width="25.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.53515625" customWidth="1"/>
+    <col min="2" max="2" width="25.15234375" customWidth="1"/>
+    <col min="3" max="3" width="31.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -661,7 +661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -678,7 +678,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -698,7 +698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -718,7 +718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -735,7 +735,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -752,7 +752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -766,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -794,7 +794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -808,7 +808,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -830,13 +830,13 @@
         <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -850,7 +850,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>44</v>
       </c>
@@ -864,7 +864,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -878,7 +878,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>50</v>
       </c>
@@ -892,7 +892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>53</v>
       </c>
@@ -900,13 +900,13 @@
         <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E18">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -920,7 +920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>57</v>
       </c>
@@ -934,7 +934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>60</v>
       </c>
@@ -948,26 +948,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
+        <v>85</v>
+      </c>
+      <c r="B22" t="s">
         <v>86</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>87</v>
       </c>
-      <c r="C22" t="s">
-        <v>88</v>
-      </c>
       <c r="F22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
         <v>17</v>
@@ -976,26 +976,26 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
         <v>65</v>
       </c>
-      <c r="B24" t="s">
-        <v>66</v>
-      </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
         <v>68</v>
-      </c>
-      <c r="B25" t="s">
-        <v>69</v>
       </c>
       <c r="C25" t="s">
         <v>14</v>
@@ -1004,12 +1004,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
         <v>70</v>
-      </c>
-      <c r="B26" t="s">
-        <v>71</v>
       </c>
       <c r="C26" t="s">
         <v>14</v>
@@ -1018,40 +1018,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
         <v>72</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>66</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A28" t="s">
         <v>73</v>
       </c>
-      <c r="C27" t="s">
-        <v>67</v>
-      </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" t="s">
         <v>74</v>
       </c>
-      <c r="B28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="F28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A29" t="s">
         <v>75</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>76</v>
-      </c>
-      <c r="B29" t="s">
-        <v>77</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
@@ -1060,12 +1060,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
+        <v>77</v>
+      </c>
+      <c r="B30" t="s">
         <v>78</v>
-      </c>
-      <c r="B30" t="s">
-        <v>79</v>
       </c>
       <c r="C30" t="s">
         <v>14</v>
@@ -1074,12 +1074,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" t="s">
         <v>80</v>
-      </c>
-      <c r="B31" t="s">
-        <v>81</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>

</xml_diff>